<commit_message>
Added Parasitic losses, Euler Implicit simulation
</commit_message>
<xml_diff>
--- a/reskit/solar/workflows/CSP_data/CSP_database.xlsx
+++ b/reskit/solar/workflows/CSP_data/CSP_database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d.franzmann\Code\RESKit\reskit\solar\workflows\CSP_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20533A2C-FBE7-492B-8FFC-01D69B2992C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2615EF-61D3-4CF0-9004-B7A8BC2ACD66}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EF8FF396-6CE6-4D67-BA8C-A21BECB15794}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16920" xr2:uid="{EF8FF396-6CE6-4D67-BA8C-A21BECB15794}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="78">
   <si>
     <t>Parameter</t>
   </si>
@@ -78,9 +78,6 @@
     <t>b4</t>
   </si>
   <si>
-    <t>TM_plant</t>
-  </si>
-  <si>
     <t>maxHTFTemperature</t>
   </si>
   <si>
@@ -99,9 +96,6 @@
     <t>song2013</t>
   </si>
   <si>
-    <t>Validation 1</t>
-  </si>
-  <si>
     <t>Unit</t>
   </si>
   <si>
@@ -189,17 +183,98 @@
     <t>Gafurov, Greenius</t>
   </si>
   <si>
-    <t>Gafurov, losses from Grrnius</t>
-  </si>
-  <si>
     <t>dataset name</t>
+  </si>
+  <si>
+    <t>Gafurov, losses from Greenius</t>
+  </si>
+  <si>
+    <t>relTMplant</t>
+  </si>
+  <si>
+    <t>heatlossfactor</t>
+  </si>
+  <si>
+    <t>Validation_2</t>
+  </si>
+  <si>
+    <t>Validation_1</t>
+  </si>
+  <si>
+    <t>heatlossconstant</t>
+  </si>
+  <si>
+    <t>add_losses_coefficient</t>
+  </si>
+  <si>
+    <t>W/m^2K</t>
+  </si>
+  <si>
+    <t>Validation_3</t>
+  </si>
+  <si>
+    <t>Validation_4</t>
+  </si>
+  <si>
+    <t>Validation_5</t>
+  </si>
+  <si>
+    <t>discretizationmethod</t>
+  </si>
+  <si>
+    <t>Simulation Method</t>
+  </si>
+  <si>
+    <t>euler explicit</t>
+  </si>
+  <si>
+    <t>euler implicit</t>
+  </si>
+  <si>
+    <t>Validation_6</t>
+  </si>
+  <si>
+    <t>Validation_7</t>
+  </si>
+  <si>
+    <t>I_DNI_nom</t>
+  </si>
+  <si>
+    <t>PL_plant_fix</t>
+  </si>
+  <si>
+    <t>PL_sf_track</t>
+  </si>
+  <si>
+    <t>PL_sf_pumping</t>
+  </si>
+  <si>
+    <t>PL_plant_pumping</t>
+  </si>
+  <si>
+    <t>PL_plant_other</t>
+  </si>
+  <si>
+    <t>W/m^2</t>
+  </si>
+  <si>
+    <t>Validation_8</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>PL from Gafurov</t>
+  </si>
+  <si>
+    <t>Parasitic losses</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,13 +282,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -228,12 +315,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -548,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40AE3422-B05C-445F-BBB4-0860483AF0A6}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,111 +653,239 @@
     <col min="3" max="3" width="18.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="27.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2" t="s">
+        <v>65</v>
+      </c>
+      <c r="K2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>18</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B3" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" t="s">
+        <v>41</v>
+      </c>
+      <c r="L3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D4">
         <v>8.8400000000000002E-4</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="8">
         <v>8.4924000000000002E-5</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="1">
+        <v>8.4924000000000002E-5</v>
+      </c>
+      <c r="G4" s="1">
+        <v>8.4924000000000002E-5</v>
+      </c>
+      <c r="H4" s="1">
+        <v>8.4924000000000002E-5</v>
+      </c>
+      <c r="I4" s="1">
+        <v>8.4924000000000002E-5</v>
+      </c>
+      <c r="J4" s="1">
+        <v>8.4924000000000002E-5</v>
+      </c>
+      <c r="K4" s="1">
+        <v>8.4924000000000002E-5</v>
+      </c>
+      <c r="L4" s="1">
+        <v>8.4924000000000002E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D5">
         <v>5.3690000000000003E-5</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="8">
         <v>3.1093000000000002E-5</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="1">
+        <v>3.1093000000000002E-5</v>
+      </c>
+      <c r="G5" s="1">
+        <v>3.1093000000000002E-5</v>
+      </c>
+      <c r="H5" s="1">
+        <v>3.1093000000000002E-5</v>
+      </c>
+      <c r="I5" s="1">
+        <v>3.1093000000000002E-5</v>
+      </c>
+      <c r="J5" s="1">
+        <v>3.1093000000000002E-5</v>
+      </c>
+      <c r="K5" s="1">
+        <v>3.1093000000000002E-5</v>
+      </c>
+      <c r="L5" s="1">
+        <v>3.1093000000000002E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" s="7">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -673,33 +893,75 @@
         <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D7">
         <v>0.74199999999999999</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="7">
         <v>0.82699999999999996</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="G7">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="H7">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="I7">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="J7">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="K7">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="L7">
+        <v>0.82699999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D8">
         <v>909060</v>
       </c>
-      <c r="E8">
-        <v>1581372</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" s="7">
+        <v>1372800</v>
+      </c>
+      <c r="F8">
+        <v>1372800</v>
+      </c>
+      <c r="G8">
+        <v>1372800</v>
+      </c>
+      <c r="H8">
+        <v>1372800</v>
+      </c>
+      <c r="I8">
+        <v>1372800</v>
+      </c>
+      <c r="J8">
+        <v>1372800</v>
+      </c>
+      <c r="K8">
+        <v>1372800</v>
+      </c>
+      <c r="L8">
+        <v>1372800</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -707,21 +969,22 @@
         <v>1</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D9">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D10">
         <v>14</v>
@@ -729,16 +992,37 @@
       <c r="E10">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>14</v>
+      </c>
+      <c r="G10">
+        <v>14</v>
+      </c>
+      <c r="H10">
+        <v>14</v>
+      </c>
+      <c r="I10">
+        <v>14</v>
+      </c>
+      <c r="J10">
+        <v>14</v>
+      </c>
+      <c r="K10">
+        <v>14</v>
+      </c>
+      <c r="L10">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -746,16 +1030,37 @@
       <c r="E11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D12">
         <v>2.4209999999999999E-2</v>
@@ -763,16 +1068,37 @@
       <c r="E12">
         <v>2.4209999999999999E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>2.4209999999999999E-2</v>
+      </c>
+      <c r="G12">
+        <v>2.4209999999999999E-2</v>
+      </c>
+      <c r="H12">
+        <v>2.4209999999999999E-2</v>
+      </c>
+      <c r="I12">
+        <v>2.4209999999999999E-2</v>
+      </c>
+      <c r="J12">
+        <v>2.4209999999999999E-2</v>
+      </c>
+      <c r="K12">
+        <v>2.4209999999999999E-2</v>
+      </c>
+      <c r="L12">
+        <v>2.4209999999999999E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D13" s="1">
         <v>2.461E-5</v>
@@ -780,16 +1106,37 @@
       <c r="E13" s="1">
         <v>2.461E-5</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="1">
+        <v>2.461E-5</v>
+      </c>
+      <c r="G13" s="1">
+        <v>2.461E-5</v>
+      </c>
+      <c r="H13" s="1">
+        <v>2.461E-5</v>
+      </c>
+      <c r="I13" s="1">
+        <v>2.461E-5</v>
+      </c>
+      <c r="J13" s="1">
+        <v>2.461E-5</v>
+      </c>
+      <c r="K13" s="1">
+        <v>2.461E-5</v>
+      </c>
+      <c r="L13" s="1">
+        <v>2.461E-5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D14" s="1">
         <v>1.5559999999999999E-7</v>
@@ -797,16 +1144,37 @@
       <c r="E14" s="1">
         <v>1.5559999999999999E-7</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="1">
+        <v>1.5559999999999999E-7</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1.5559999999999999E-7</v>
+      </c>
+      <c r="H14" s="1">
+        <v>1.5559999999999999E-7</v>
+      </c>
+      <c r="I14" s="1">
+        <v>1.5559999999999999E-7</v>
+      </c>
+      <c r="J14" s="1">
+        <v>1.5559999999999999E-7</v>
+      </c>
+      <c r="K14" s="1">
+        <v>1.5559999999999999E-7</v>
+      </c>
+      <c r="L14" s="1">
+        <v>1.5559999999999999E-7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="D15" s="1">
         <v>1.1700000000000001E-9</v>
@@ -814,8 +1182,29 @@
       <c r="E15" s="1">
         <v>1.1700000000000001E-9</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" s="1">
+        <v>1.1700000000000001E-9</v>
+      </c>
+      <c r="G15" s="1">
+        <v>1.1700000000000001E-9</v>
+      </c>
+      <c r="H15" s="1">
+        <v>1.1700000000000001E-9</v>
+      </c>
+      <c r="I15" s="1">
+        <v>1.1700000000000001E-9</v>
+      </c>
+      <c r="J15" s="1">
+        <v>1.1700000000000001E-9</v>
+      </c>
+      <c r="K15" s="1">
+        <v>1.1700000000000001E-9</v>
+      </c>
+      <c r="L15" s="1">
+        <v>1.1700000000000001E-9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -823,164 +1212,749 @@
         <v>1</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D16">
         <v>0.38300000000000001</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="8">
         <v>0.30509999999999998</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="1">
+        <v>0.30509999999999998</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0.30509999999999998</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0.30509999999999998</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0.30509999999999998</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0.30509999999999998</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0.30509999999999998</v>
+      </c>
+      <c r="L16" s="1">
+        <v>0.30509999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D17">
         <f>1000*D8*D7</f>
         <v>674522520</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0</v>
+      </c>
+      <c r="K17" s="1">
+        <v>0</v>
+      </c>
+      <c r="L17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="5">
         <v>0.97</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="4">
+        <v>0.97</v>
+      </c>
+      <c r="G18" s="4">
+        <v>0.97</v>
+      </c>
+      <c r="H18" s="4">
+        <v>0.97</v>
+      </c>
+      <c r="I18" s="4">
+        <v>0.97</v>
+      </c>
+      <c r="J18" s="4">
+        <v>0.97</v>
+      </c>
+      <c r="K18" s="4">
+        <v>0.97</v>
+      </c>
+      <c r="L18" s="4">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+      <c r="G19" s="7">
+        <v>0.108</v>
+      </c>
+      <c r="H19">
+        <v>0.108</v>
+      </c>
+      <c r="I19">
+        <v>0.108</v>
+      </c>
+      <c r="J19">
+        <v>0.108</v>
+      </c>
+      <c r="K19">
+        <v>0.108</v>
+      </c>
+      <c r="L19">
+        <v>0.108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" s="7">
+        <v>1.81</v>
+      </c>
+      <c r="G20" s="7">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21" s="8">
+        <v>5500000</v>
+      </c>
+      <c r="H21" s="1">
+        <v>5500000</v>
+      </c>
+      <c r="I21" s="1">
+        <v>5500000</v>
+      </c>
+      <c r="J21" s="1">
+        <v>5500000</v>
+      </c>
+      <c r="K21" s="1">
+        <v>5500000</v>
+      </c>
+      <c r="L21" s="1">
+        <v>5500000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22">
+        <v>600</v>
+      </c>
+      <c r="E22">
+        <v>600</v>
+      </c>
+      <c r="F22">
+        <v>600</v>
+      </c>
+      <c r="G22">
+        <v>600</v>
+      </c>
+      <c r="H22">
+        <v>600</v>
+      </c>
+      <c r="I22">
+        <v>600</v>
+      </c>
+      <c r="J22">
+        <v>600</v>
+      </c>
+      <c r="K22">
+        <v>600</v>
+      </c>
+      <c r="L22">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D23">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="E23">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="F23">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="G23">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="H23">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="I23">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="J23">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="K23">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="L23">
+        <v>5.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="E24">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="F24">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="G24">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="H24">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="I24">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="J24">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="K24">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="L24">
+        <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25">
+        <v>0.05</v>
+      </c>
+      <c r="E25">
+        <v>0.05</v>
+      </c>
+      <c r="F25">
+        <v>0.05</v>
+      </c>
+      <c r="G25">
+        <v>0.05</v>
+      </c>
+      <c r="H25">
+        <v>0.05</v>
+      </c>
+      <c r="I25">
+        <v>0.05</v>
+      </c>
+      <c r="J25">
+        <v>0.05</v>
+      </c>
+      <c r="K25">
+        <v>0.05</v>
+      </c>
+      <c r="L25">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D26">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E26">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F26">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G26">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="H26">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="I26">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="J26">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="K26">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="L26">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D27">
+        <v>1.9E-2</v>
+      </c>
+      <c r="E27">
+        <v>1.9E-2</v>
+      </c>
+      <c r="F27">
+        <v>1.9E-2</v>
+      </c>
+      <c r="G27">
+        <v>1.9E-2</v>
+      </c>
+      <c r="H27">
+        <v>1.9E-2</v>
+      </c>
+      <c r="I27">
+        <v>1.9E-2</v>
+      </c>
+      <c r="J27">
+        <v>1.9E-2</v>
+      </c>
+      <c r="K27">
+        <v>1.9E-2</v>
+      </c>
+      <c r="L27">
+        <v>1.9E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28">
+        <v>1100</v>
+      </c>
+      <c r="E28" s="4">
+        <v>1100</v>
+      </c>
+      <c r="F28" s="4">
+        <v>1100</v>
+      </c>
+      <c r="G28" s="4">
+        <v>1100</v>
+      </c>
+      <c r="H28" s="5">
+        <v>3688</v>
+      </c>
+      <c r="I28" s="6">
+        <v>3688</v>
+      </c>
+      <c r="J28" s="5">
+        <v>1100</v>
+      </c>
+      <c r="K28" s="5">
+        <v>3688</v>
+      </c>
+      <c r="L28" s="6">
+        <v>3688</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="3" t="s">
+      <c r="B29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29">
+        <v>385</v>
+      </c>
+      <c r="E29" s="4">
+        <v>385</v>
+      </c>
+      <c r="F29" s="4">
+        <v>385</v>
+      </c>
+      <c r="G29" s="4">
+        <v>385</v>
+      </c>
+      <c r="H29" s="6">
+        <v>385</v>
+      </c>
+      <c r="I29" s="6">
+        <v>385</v>
+      </c>
+      <c r="J29" s="6">
+        <v>385</v>
+      </c>
+      <c r="K29" s="6">
+        <v>385</v>
+      </c>
+      <c r="L29" s="6">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30">
+        <v>15</v>
+      </c>
+      <c r="E30" s="5">
+        <v>60</v>
+      </c>
+      <c r="F30" s="4">
+        <v>60</v>
+      </c>
+      <c r="G30" s="4">
+        <v>60</v>
+      </c>
+      <c r="H30" s="4">
+        <v>60</v>
+      </c>
+      <c r="I30" s="4">
+        <v>60</v>
+      </c>
+      <c r="J30" s="4">
+        <v>60</v>
+      </c>
+      <c r="K30" s="4">
+        <v>60</v>
+      </c>
+      <c r="L30" s="4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D31">
+        <v>295</v>
+      </c>
+      <c r="E31">
+        <v>295</v>
+      </c>
+      <c r="F31">
+        <v>295</v>
+      </c>
+      <c r="G31">
+        <v>295</v>
+      </c>
+      <c r="H31">
+        <v>295</v>
+      </c>
+      <c r="I31">
+        <v>295</v>
+      </c>
+      <c r="J31">
+        <v>295</v>
+      </c>
+      <c r="K31">
+        <v>295</v>
+      </c>
+      <c r="L31">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D32" t="s">
+        <v>63</v>
+      </c>
+      <c r="E32" t="s">
+        <v>63</v>
+      </c>
+      <c r="F32" t="s">
+        <v>63</v>
+      </c>
+      <c r="G32" t="s">
+        <v>63</v>
+      </c>
+      <c r="H32" t="s">
+        <v>63</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="J32" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="K32" t="s">
+        <v>63</v>
+      </c>
+      <c r="L32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="1">
-        <v>1000000000</v>
-      </c>
-      <c r="E19" s="1">
-        <v>1000000000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20">
-        <v>385</v>
-      </c>
-      <c r="E20" s="4">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21">
-        <v>15</v>
-      </c>
-      <c r="E21" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22">
-        <v>295</v>
-      </c>
-      <c r="E22">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D23" s="3" t="s">
+      <c r="D33" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E33" t="s">
+        <v>43</v>
+      </c>
+      <c r="F33" t="s">
+        <v>43</v>
+      </c>
+      <c r="G33" t="s">
+        <v>43</v>
+      </c>
+      <c r="H33" t="s">
+        <v>43</v>
+      </c>
+      <c r="I33" t="s">
+        <v>43</v>
+      </c>
+      <c r="J33" t="s">
+        <v>43</v>
+      </c>
+      <c r="K33" t="s">
+        <v>43</v>
+      </c>
+      <c r="L33" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" t="s">
+        <v>46</v>
+      </c>
+      <c r="E34" t="s">
+        <v>46</v>
+      </c>
+      <c r="F34" t="s">
+        <v>46</v>
+      </c>
+      <c r="G34" t="s">
+        <v>46</v>
+      </c>
+      <c r="H34" t="s">
+        <v>46</v>
+      </c>
+      <c r="I34" t="s">
+        <v>46</v>
+      </c>
+      <c r="J34" t="s">
+        <v>46</v>
+      </c>
+      <c r="K34" t="s">
+        <v>46</v>
+      </c>
+      <c r="L34" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35" t="s">
         <v>50</v>
       </c>
-      <c r="E23" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24" t="s">
-        <v>48</v>
-      </c>
-      <c r="E24" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D25" t="s">
-        <v>51</v>
-      </c>
+      <c r="K35" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>75</v>
+      </c>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="9"/>
+      <c r="L36" s="9"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
added testing functions and elevation calc
</commit_message>
<xml_diff>
--- a/reskit/solar/workflows/CSP_data/CSP_database.xlsx
+++ b/reskit/solar/workflows/CSP_data/CSP_database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d.franzmann\Code\RESKit\reskit\solar\workflows\CSP_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065C8412-E4F6-4174-9CC6-CD3B555ABBEE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2FBE199-4E78-44F9-B8C1-30C190CBCA0C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16920" xr2:uid="{EF8FF396-6CE6-4D67-BA8C-A21BECB15794}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="83">
   <si>
     <t>Parameter</t>
   </si>
@@ -192,18 +192,12 @@
     <t>relTMplant</t>
   </si>
   <si>
-    <t>heatlossfactor</t>
-  </si>
-  <si>
     <t>Validation_2</t>
   </si>
   <si>
     <t>Validation_1</t>
   </si>
   <si>
-    <t>heatlossconstant</t>
-  </si>
-  <si>
     <t>add_losses_coefficient</t>
   </si>
   <si>
@@ -283,13 +277,19 @@
   </si>
   <si>
     <t>genral</t>
+  </si>
+  <si>
+    <t>Dataset1</t>
+  </si>
+  <si>
+    <t>Validation_10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -299,6 +299,12 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -330,7 +336,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -341,6 +347,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -655,10 +664,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40AE3422-B05C-445F-BBB4-0860483AF0A6}">
-  <dimension ref="A1:M38"/>
+  <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,9 +682,10 @@
     <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="13" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -686,34 +699,40 @@
         <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" t="s">
         <v>58</v>
       </c>
-      <c r="H1" t="s">
-        <v>59</v>
-      </c>
-      <c r="I1" t="s">
-        <v>60</v>
-      </c>
       <c r="J1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="M1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="N1" t="s">
+        <v>82</v>
+      </c>
+      <c r="O1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -727,34 +746,40 @@
         <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I2" t="s">
         <v>58</v>
       </c>
-      <c r="H2" t="s">
-        <v>59</v>
-      </c>
-      <c r="I2" t="s">
-        <v>60</v>
-      </c>
       <c r="J2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="M2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="N2" t="s">
+        <v>82</v>
+      </c>
+      <c r="O2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -794,8 +819,14 @@
       <c r="M3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -835,8 +866,12 @@
       <c r="M4" s="1">
         <v>8.4924000000000002E-5</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4" s="1">
+        <v>8.4924000000000002E-5</v>
+      </c>
+      <c r="O4" s="1"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -876,8 +911,12 @@
       <c r="M5" s="1">
         <v>3.1093000000000002E-5</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5" s="1">
+        <v>3.1093000000000002E-5</v>
+      </c>
+      <c r="O5" s="1"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -917,8 +956,11 @@
       <c r="M6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -958,310 +1000,337 @@
       <c r="M7">
         <v>0.82699999999999996</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N7">
+        <v>0.82699999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>22</v>
+        <v>6</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D8">
-        <v>909060</v>
-      </c>
-      <c r="E8" s="7">
-        <v>1372800</v>
-      </c>
-      <c r="F8">
-        <v>1372800</v>
-      </c>
-      <c r="G8">
-        <v>1372800</v>
-      </c>
-      <c r="H8">
-        <v>1372800</v>
-      </c>
-      <c r="I8">
-        <v>1372800</v>
-      </c>
-      <c r="J8">
-        <v>1372800</v>
-      </c>
-      <c r="K8">
-        <v>1372800</v>
-      </c>
-      <c r="L8">
-        <v>1372800</v>
-      </c>
-      <c r="M8">
-        <v>1372800</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0.06</v>
+      </c>
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="3">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D9">
-        <v>0.06</v>
-      </c>
-      <c r="E9" s="7"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="E9">
+        <v>14</v>
+      </c>
+      <c r="F9">
+        <v>14</v>
+      </c>
+      <c r="G9">
+        <v>14</v>
+      </c>
+      <c r="H9">
+        <v>14</v>
+      </c>
+      <c r="I9">
+        <v>14</v>
+      </c>
+      <c r="J9">
+        <v>14</v>
+      </c>
+      <c r="K9">
+        <v>14</v>
+      </c>
+      <c r="L9">
+        <v>14</v>
+      </c>
+      <c r="M9">
+        <v>14</v>
+      </c>
+      <c r="N9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D10">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="G10">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="H10">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="I10">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="J10">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="K10">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="L10">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="M10">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>2.4209999999999999E-2</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>2.4209999999999999E-2</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>2.4209999999999999E-2</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>2.4209999999999999E-2</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>2.4209999999999999E-2</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>2.4209999999999999E-2</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>2.4209999999999999E-2</v>
       </c>
       <c r="K11">
-        <v>0</v>
+        <v>2.4209999999999999E-2</v>
       </c>
       <c r="L11">
-        <v>0</v>
+        <v>2.4209999999999999E-2</v>
       </c>
       <c r="M11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+        <v>2.4209999999999999E-2</v>
+      </c>
+      <c r="N11">
+        <v>2.4209999999999999E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D12">
-        <v>2.4209999999999999E-2</v>
-      </c>
-      <c r="E12">
-        <v>2.4209999999999999E-2</v>
-      </c>
-      <c r="F12">
-        <v>2.4209999999999999E-2</v>
-      </c>
-      <c r="G12">
-        <v>2.4209999999999999E-2</v>
-      </c>
-      <c r="H12">
-        <v>2.4209999999999999E-2</v>
-      </c>
-      <c r="I12">
-        <v>2.4209999999999999E-2</v>
-      </c>
-      <c r="J12">
-        <v>2.4209999999999999E-2</v>
-      </c>
-      <c r="K12">
-        <v>2.4209999999999999E-2</v>
-      </c>
-      <c r="L12">
-        <v>2.4209999999999999E-2</v>
-      </c>
-      <c r="M12">
-        <v>2.4209999999999999E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D12" s="1">
+        <v>2.461E-5</v>
+      </c>
+      <c r="E12" s="1">
+        <v>2.461E-5</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2.461E-5</v>
+      </c>
+      <c r="G12" s="1">
+        <v>2.461E-5</v>
+      </c>
+      <c r="H12" s="1">
+        <v>2.461E-5</v>
+      </c>
+      <c r="I12" s="1">
+        <v>2.461E-5</v>
+      </c>
+      <c r="J12" s="1">
+        <v>2.461E-5</v>
+      </c>
+      <c r="K12" s="1">
+        <v>2.461E-5</v>
+      </c>
+      <c r="L12" s="1">
+        <v>2.461E-5</v>
+      </c>
+      <c r="M12" s="1">
+        <v>2.461E-5</v>
+      </c>
+      <c r="N12" s="1">
+        <v>2.461E-5</v>
+      </c>
+      <c r="O12" s="1"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D13" s="1">
-        <v>2.461E-5</v>
+        <v>1.5559999999999999E-7</v>
       </c>
       <c r="E13" s="1">
-        <v>2.461E-5</v>
+        <v>1.5559999999999999E-7</v>
       </c>
       <c r="F13" s="1">
-        <v>2.461E-5</v>
+        <v>1.5559999999999999E-7</v>
       </c>
       <c r="G13" s="1">
-        <v>2.461E-5</v>
+        <v>1.5559999999999999E-7</v>
       </c>
       <c r="H13" s="1">
-        <v>2.461E-5</v>
+        <v>1.5559999999999999E-7</v>
       </c>
       <c r="I13" s="1">
-        <v>2.461E-5</v>
+        <v>1.5559999999999999E-7</v>
       </c>
       <c r="J13" s="1">
-        <v>2.461E-5</v>
+        <v>1.5559999999999999E-7</v>
       </c>
       <c r="K13" s="1">
-        <v>2.461E-5</v>
+        <v>1.5559999999999999E-7</v>
       </c>
       <c r="L13" s="1">
-        <v>2.461E-5</v>
+        <v>1.5559999999999999E-7</v>
       </c>
       <c r="M13" s="1">
-        <v>2.461E-5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1.5559999999999999E-7</v>
+      </c>
+      <c r="N13" s="1">
+        <v>1.5559999999999999E-7</v>
+      </c>
+      <c r="O13" s="1"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D14" s="1">
-        <v>1.5559999999999999E-7</v>
+        <v>1.1700000000000001E-9</v>
       </c>
       <c r="E14" s="1">
-        <v>1.5559999999999999E-7</v>
+        <v>1.1700000000000001E-9</v>
       </c>
       <c r="F14" s="1">
-        <v>1.5559999999999999E-7</v>
+        <v>1.1700000000000001E-9</v>
       </c>
       <c r="G14" s="1">
-        <v>1.5559999999999999E-7</v>
+        <v>1.1700000000000001E-9</v>
       </c>
       <c r="H14" s="1">
-        <v>1.5559999999999999E-7</v>
+        <v>1.1700000000000001E-9</v>
       </c>
       <c r="I14" s="1">
-        <v>1.5559999999999999E-7</v>
+        <v>1.1700000000000001E-9</v>
       </c>
       <c r="J14" s="1">
-        <v>1.5559999999999999E-7</v>
+        <v>1.1700000000000001E-9</v>
       </c>
       <c r="K14" s="1">
-        <v>1.5559999999999999E-7</v>
+        <v>1.1700000000000001E-9</v>
       </c>
       <c r="L14" s="1">
-        <v>1.5559999999999999E-7</v>
+        <v>1.1700000000000001E-9</v>
       </c>
       <c r="M14" s="1">
-        <v>1.5559999999999999E-7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1.1700000000000001E-9</v>
+      </c>
+      <c r="N14" s="1">
+        <v>1.1700000000000001E-9</v>
+      </c>
+      <c r="O14" s="1"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="1">
-        <v>1.1700000000000001E-9</v>
-      </c>
-      <c r="E15" s="1">
-        <v>1.1700000000000001E-9</v>
-      </c>
-      <c r="F15" s="1">
-        <v>1.1700000000000001E-9</v>
-      </c>
-      <c r="G15" s="1">
-        <v>1.1700000000000001E-9</v>
-      </c>
-      <c r="H15" s="1">
-        <v>1.1700000000000001E-9</v>
-      </c>
-      <c r="I15" s="1">
-        <v>1.1700000000000001E-9</v>
-      </c>
-      <c r="J15" s="1">
-        <v>1.1700000000000001E-9</v>
-      </c>
-      <c r="K15" s="1">
-        <v>1.1700000000000001E-9</v>
-      </c>
-      <c r="L15" s="1">
-        <v>1.1700000000000001E-9</v>
-      </c>
-      <c r="M15" s="1">
-        <v>1.1700000000000001E-9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="D15">
+        <v>909060</v>
+      </c>
+      <c r="E15" s="7">
+        <v>1372800</v>
+      </c>
+      <c r="F15">
+        <v>1372800</v>
+      </c>
+      <c r="G15">
+        <v>1372800</v>
+      </c>
+      <c r="H15">
+        <v>1372800</v>
+      </c>
+      <c r="I15">
+        <v>1372800</v>
+      </c>
+      <c r="J15">
+        <v>1372800</v>
+      </c>
+      <c r="K15">
+        <v>1372800</v>
+      </c>
+      <c r="L15">
+        <v>1372800</v>
+      </c>
+      <c r="M15">
+        <v>1372800</v>
+      </c>
+      <c r="N15">
+        <v>1372800</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -1271,38 +1340,42 @@
       <c r="C16" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="10">
         <v>0.38300000000000001</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="11">
         <v>0.30509999999999998</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="10">
         <v>0.30509999999999998</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16" s="10">
         <v>0.30509999999999998</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16" s="10">
         <v>0.30509999999999998</v>
       </c>
-      <c r="I16" s="1">
+      <c r="I16" s="10">
         <v>0.30509999999999998</v>
       </c>
-      <c r="J16" s="1">
+      <c r="J16" s="10">
         <v>0.30509999999999998</v>
       </c>
-      <c r="K16" s="1">
+      <c r="K16" s="10">
         <v>0.30509999999999998</v>
       </c>
-      <c r="L16" s="1">
+      <c r="L16" s="10">
         <v>0.30509999999999998</v>
       </c>
-      <c r="M16" s="1">
+      <c r="M16" s="10">
         <v>0.30509999999999998</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N16" s="11">
+        <v>0.434</v>
+      </c>
+      <c r="O16" s="10"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1312,39 +1385,43 @@
       <c r="C17" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D17">
-        <f>1000*D8*D7</f>
+      <c r="D17" s="10">
+        <f>1000*D15*D7</f>
         <v>674522520</v>
       </c>
-      <c r="E17" s="1">
-        <v>0</v>
-      </c>
-      <c r="F17" s="1">
-        <v>0</v>
-      </c>
-      <c r="G17" s="1">
-        <v>0</v>
-      </c>
-      <c r="H17" s="1">
-        <v>0</v>
-      </c>
-      <c r="I17" s="1">
-        <v>0</v>
-      </c>
-      <c r="J17" s="1">
-        <v>0</v>
-      </c>
-      <c r="K17" s="1">
-        <v>0</v>
-      </c>
-      <c r="L17" s="1">
-        <v>0</v>
-      </c>
-      <c r="M17" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E17" s="10">
+        <v>0</v>
+      </c>
+      <c r="F17" s="10">
+        <v>0</v>
+      </c>
+      <c r="G17" s="10">
+        <v>0</v>
+      </c>
+      <c r="H17" s="10">
+        <v>0</v>
+      </c>
+      <c r="I17" s="10">
+        <v>0</v>
+      </c>
+      <c r="J17" s="10">
+        <v>0</v>
+      </c>
+      <c r="K17" s="10">
+        <v>0</v>
+      </c>
+      <c r="L17" s="10">
+        <v>0</v>
+      </c>
+      <c r="M17" s="10">
+        <v>0</v>
+      </c>
+      <c r="N17" s="10">
+        <v>0</v>
+      </c>
+      <c r="O17" s="10"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -1384,13 +1461,17 @@
       <c r="M18" s="4">
         <v>0.97</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N18" s="4">
+        <v>0.97</v>
+      </c>
+      <c r="O18" s="4"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>34</v>
@@ -1425,10 +1506,13 @@
       <c r="M19">
         <v>0.108</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N19">
+        <v>0.108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>45</v>
@@ -1437,160 +1521,174 @@
         <v>34</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20" s="7">
-        <v>1.81</v>
-      </c>
-      <c r="G20" s="7">
-        <v>1</v>
-      </c>
-      <c r="H20">
-        <v>1</v>
-      </c>
-      <c r="I20">
-        <v>1</v>
-      </c>
-      <c r="J20">
-        <v>1</v>
-      </c>
-      <c r="K20">
-        <v>1</v>
-      </c>
-      <c r="L20">
-        <v>1</v>
-      </c>
-      <c r="M20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20" s="8">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0</v>
+      </c>
+      <c r="J20" s="1">
+        <v>0</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0</v>
+      </c>
+      <c r="L20" s="1">
+        <v>0</v>
+      </c>
+      <c r="M20" s="1">
+        <v>0</v>
+      </c>
+      <c r="N20" s="1">
+        <v>0</v>
+      </c>
+      <c r="O20" s="1"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>34</v>
+        <v>75</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21" s="8">
-        <v>5500000</v>
-      </c>
-      <c r="H21" s="1">
-        <v>5500000</v>
-      </c>
-      <c r="I21" s="1">
-        <v>5500000</v>
-      </c>
-      <c r="J21" s="1">
-        <v>5500000</v>
-      </c>
-      <c r="K21" s="1">
-        <v>5500000</v>
-      </c>
-      <c r="L21" s="1">
-        <v>5500000</v>
-      </c>
-      <c r="M21" s="1">
-        <v>5500000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+        <v>600</v>
+      </c>
+      <c r="G21">
+        <v>600</v>
+      </c>
+      <c r="H21">
+        <v>600</v>
+      </c>
+      <c r="I21">
+        <v>600</v>
+      </c>
+      <c r="J21">
+        <v>600</v>
+      </c>
+      <c r="K21">
+        <v>600</v>
+      </c>
+      <c r="L21">
+        <v>600</v>
+      </c>
+      <c r="M21">
+        <v>600</v>
+      </c>
+      <c r="N21">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>45</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>34</v>
+        <v>75</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22" s="8">
-        <v>0</v>
-      </c>
-      <c r="H22" s="1">
-        <v>0</v>
-      </c>
-      <c r="I22" s="1">
-        <v>0</v>
-      </c>
-      <c r="J22" s="1">
-        <v>0</v>
-      </c>
-      <c r="K22" s="1">
-        <v>0</v>
-      </c>
-      <c r="L22" s="1">
-        <v>0</v>
-      </c>
-      <c r="M22" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="G22">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="H22">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="I22">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="J22">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="K22">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="L22">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="M22">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="N22">
+        <v>5.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>67</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D23">
-        <v>600</v>
+        <v>2.5999999999999999E-3</v>
       </c>
       <c r="E23">
-        <v>600</v>
+        <v>2.5999999999999999E-3</v>
       </c>
       <c r="F23">
-        <v>600</v>
+        <v>2.5999999999999999E-3</v>
       </c>
       <c r="G23">
-        <v>600</v>
+        <v>2.5999999999999999E-3</v>
       </c>
       <c r="H23">
-        <v>600</v>
+        <v>2.5999999999999999E-3</v>
       </c>
       <c r="I23">
-        <v>600</v>
+        <v>2.5999999999999999E-3</v>
       </c>
       <c r="J23">
-        <v>600</v>
+        <v>2.5999999999999999E-3</v>
       </c>
       <c r="K23">
-        <v>600</v>
-      </c>
-      <c r="L23">
-        <v>600</v>
-      </c>
-      <c r="M23">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="L23" s="7">
+        <v>1.6E-2</v>
+      </c>
+      <c r="M23" s="9">
+        <v>1.6E-2</v>
+      </c>
+      <c r="N23" s="9">
+        <v>1.6E-2</v>
+      </c>
+      <c r="O23" s="9"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>68</v>
       </c>
@@ -1598,40 +1696,44 @@
         <v>45</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D24">
-        <v>5.4999999999999997E-3</v>
+        <v>0.05</v>
       </c>
       <c r="E24">
-        <v>5.4999999999999997E-3</v>
+        <v>0.05</v>
       </c>
       <c r="F24">
-        <v>5.4999999999999997E-3</v>
+        <v>0.05</v>
       </c>
       <c r="G24">
-        <v>5.4999999999999997E-3</v>
+        <v>0.05</v>
       </c>
       <c r="H24">
-        <v>5.4999999999999997E-3</v>
+        <v>0.05</v>
       </c>
       <c r="I24">
-        <v>5.4999999999999997E-3</v>
+        <v>0.05</v>
       </c>
       <c r="J24">
-        <v>5.4999999999999997E-3</v>
+        <v>0.05</v>
       </c>
       <c r="K24">
-        <v>5.4999999999999997E-3</v>
-      </c>
-      <c r="L24">
-        <v>5.4999999999999997E-3</v>
-      </c>
-      <c r="M24">
-        <v>5.4999999999999997E-3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0.05</v>
+      </c>
+      <c r="L24" s="7">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="M24" s="7">
+        <v>1.15E-2</v>
+      </c>
+      <c r="N24" s="12">
+        <v>1.15E-2</v>
+      </c>
+      <c r="O24" s="9"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>69</v>
       </c>
@@ -1639,40 +1741,43 @@
         <v>45</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D25">
-        <v>2.5999999999999999E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="E25">
-        <v>2.5999999999999999E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="F25">
-        <v>2.5999999999999999E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="G25">
-        <v>2.5999999999999999E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H25">
-        <v>2.5999999999999999E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="I25">
-        <v>2.5999999999999999E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="J25">
-        <v>2.5999999999999999E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="K25">
-        <v>2.5999999999999999E-3</v>
-      </c>
-      <c r="L25" s="7">
-        <v>1.6E-2</v>
-      </c>
-      <c r="M25" s="9">
-        <v>1.6E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="L25">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="M25">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="N25">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>70</v>
       </c>
@@ -1680,165 +1785,180 @@
         <v>45</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D26">
-        <v>0.05</v>
+        <v>1.9E-2</v>
       </c>
       <c r="E26">
-        <v>0.05</v>
+        <v>1.9E-2</v>
       </c>
       <c r="F26">
-        <v>0.05</v>
+        <v>1.9E-2</v>
       </c>
       <c r="G26">
-        <v>0.05</v>
+        <v>1.9E-2</v>
       </c>
       <c r="H26">
-        <v>0.05</v>
+        <v>1.9E-2</v>
       </c>
       <c r="I26">
-        <v>0.05</v>
+        <v>1.9E-2</v>
       </c>
       <c r="J26">
-        <v>0.05</v>
+        <v>1.9E-2</v>
       </c>
       <c r="K26">
-        <v>0.05</v>
-      </c>
-      <c r="L26" s="7">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="M26" s="7">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1.9E-2</v>
+      </c>
+      <c r="L26">
+        <v>1.9E-2</v>
+      </c>
+      <c r="M26">
+        <v>1.9E-2</v>
+      </c>
+      <c r="N26">
+        <v>1.9E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>77</v>
+        <v>35</v>
       </c>
       <c r="D27">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="E27">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="F27">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="G27">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="H27">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="I27">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="J27">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="K27">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="L27">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="M27">
-        <v>3.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1100</v>
+      </c>
+      <c r="E27" s="4">
+        <v>1100</v>
+      </c>
+      <c r="F27" s="4">
+        <v>1100</v>
+      </c>
+      <c r="G27" s="4">
+        <v>1100</v>
+      </c>
+      <c r="H27" s="5">
+        <v>3688</v>
+      </c>
+      <c r="I27" s="6">
+        <v>3688</v>
+      </c>
+      <c r="J27" s="5">
+        <v>1100</v>
+      </c>
+      <c r="K27" s="5">
+        <v>3688</v>
+      </c>
+      <c r="L27" s="6">
+        <v>3688</v>
+      </c>
+      <c r="M27" s="6">
+        <v>3688</v>
+      </c>
+      <c r="N27" s="6">
+        <v>3688</v>
+      </c>
+      <c r="O27" s="6"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>77</v>
+        <v>36</v>
       </c>
       <c r="D28">
-        <v>1.9E-2</v>
-      </c>
-      <c r="E28">
-        <v>1.9E-2</v>
-      </c>
-      <c r="F28">
-        <v>1.9E-2</v>
-      </c>
-      <c r="G28">
-        <v>1.9E-2</v>
-      </c>
-      <c r="H28">
-        <v>1.9E-2</v>
-      </c>
-      <c r="I28">
-        <v>1.9E-2</v>
-      </c>
-      <c r="J28">
-        <v>1.9E-2</v>
-      </c>
-      <c r="K28">
-        <v>1.9E-2</v>
-      </c>
-      <c r="L28">
-        <v>1.9E-2</v>
-      </c>
-      <c r="M28">
-        <v>1.9E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+        <v>385</v>
+      </c>
+      <c r="E28" s="4">
+        <v>385</v>
+      </c>
+      <c r="F28" s="4">
+        <v>385</v>
+      </c>
+      <c r="G28" s="4">
+        <v>385</v>
+      </c>
+      <c r="H28" s="6">
+        <v>385</v>
+      </c>
+      <c r="I28" s="6">
+        <v>385</v>
+      </c>
+      <c r="J28" s="6">
+        <v>385</v>
+      </c>
+      <c r="K28" s="6">
+        <v>385</v>
+      </c>
+      <c r="L28" s="6">
+        <v>385</v>
+      </c>
+      <c r="M28" s="6">
+        <v>385</v>
+      </c>
+      <c r="N28" s="6">
+        <v>385</v>
+      </c>
+      <c r="O28" s="6"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D29">
-        <v>1100</v>
-      </c>
-      <c r="E29" s="4">
-        <v>1100</v>
+        <v>15</v>
+      </c>
+      <c r="E29" s="5">
+        <v>60</v>
       </c>
       <c r="F29" s="4">
-        <v>1100</v>
+        <v>60</v>
       </c>
       <c r="G29" s="4">
-        <v>1100</v>
-      </c>
-      <c r="H29" s="5">
-        <v>3688</v>
-      </c>
-      <c r="I29" s="6">
-        <v>3688</v>
-      </c>
-      <c r="J29" s="5">
-        <v>1100</v>
-      </c>
-      <c r="K29" s="5">
-        <v>3688</v>
-      </c>
-      <c r="L29" s="6">
-        <v>3688</v>
-      </c>
-      <c r="M29" s="6">
-        <v>3688</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="H29" s="4">
+        <v>60</v>
+      </c>
+      <c r="I29" s="4">
+        <v>60</v>
+      </c>
+      <c r="J29" s="4">
+        <v>60</v>
+      </c>
+      <c r="K29" s="4">
+        <v>60</v>
+      </c>
+      <c r="L29" s="4">
+        <v>60</v>
+      </c>
+      <c r="M29" s="4">
+        <v>60</v>
+      </c>
+      <c r="N29" s="4">
+        <v>60</v>
+      </c>
+      <c r="O29" s="4"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>26</v>
@@ -1847,203 +1967,218 @@
         <v>36</v>
       </c>
       <c r="D30">
-        <v>385</v>
-      </c>
-      <c r="E30" s="4">
-        <v>385</v>
-      </c>
-      <c r="F30" s="4">
-        <v>385</v>
-      </c>
-      <c r="G30" s="4">
-        <v>385</v>
-      </c>
-      <c r="H30" s="6">
-        <v>385</v>
-      </c>
-      <c r="I30" s="6">
-        <v>385</v>
-      </c>
-      <c r="J30" s="6">
-        <v>385</v>
-      </c>
-      <c r="K30" s="6">
-        <v>385</v>
-      </c>
-      <c r="L30" s="6">
-        <v>385</v>
-      </c>
-      <c r="M30" s="6">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+      <c r="E30">
+        <v>295</v>
+      </c>
+      <c r="F30">
+        <v>295</v>
+      </c>
+      <c r="G30">
+        <v>295</v>
+      </c>
+      <c r="H30">
+        <v>295</v>
+      </c>
+      <c r="I30">
+        <v>295</v>
+      </c>
+      <c r="J30">
+        <v>295</v>
+      </c>
+      <c r="K30">
+        <v>295</v>
+      </c>
+      <c r="L30">
+        <v>295</v>
+      </c>
+      <c r="M30">
+        <v>295</v>
+      </c>
+      <c r="N30">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>15</v>
+        <v>78</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="C31" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D31">
+        <v>40</v>
+      </c>
+      <c r="E31">
+        <v>40</v>
+      </c>
+      <c r="F31">
+        <v>40</v>
+      </c>
+      <c r="G31">
+        <v>40</v>
+      </c>
+      <c r="H31">
+        <v>40</v>
+      </c>
+      <c r="I31">
+        <v>40</v>
+      </c>
+      <c r="J31">
+        <v>40</v>
+      </c>
+      <c r="K31">
+        <v>40</v>
+      </c>
+      <c r="L31">
+        <v>40</v>
+      </c>
+      <c r="M31">
+        <v>40</v>
+      </c>
+      <c r="N31">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" t="s">
+        <v>61</v>
+      </c>
+      <c r="E32" t="s">
+        <v>61</v>
+      </c>
+      <c r="F32" t="s">
+        <v>61</v>
+      </c>
+      <c r="G32" t="s">
+        <v>61</v>
+      </c>
+      <c r="H32" t="s">
+        <v>61</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="J32" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="K32" t="s">
+        <v>61</v>
+      </c>
+      <c r="L32" t="s">
+        <v>61</v>
+      </c>
+      <c r="M32" t="s">
+        <v>61</v>
+      </c>
+      <c r="N32" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E33" t="s">
+        <v>43</v>
+      </c>
+      <c r="F33" t="s">
+        <v>43</v>
+      </c>
+      <c r="G33" t="s">
+        <v>43</v>
+      </c>
+      <c r="H33" t="s">
+        <v>43</v>
+      </c>
+      <c r="I33" t="s">
+        <v>43</v>
+      </c>
+      <c r="J33" t="s">
+        <v>43</v>
+      </c>
+      <c r="K33" t="s">
+        <v>43</v>
+      </c>
+      <c r="L33" t="s">
+        <v>43</v>
+      </c>
+      <c r="M33" t="s">
+        <v>43</v>
+      </c>
+      <c r="N33" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="D31">
-        <v>15</v>
-      </c>
-      <c r="E31" s="5">
-        <v>60</v>
-      </c>
-      <c r="F31" s="4">
-        <v>60</v>
-      </c>
-      <c r="G31" s="4">
-        <v>60</v>
-      </c>
-      <c r="H31" s="4">
-        <v>60</v>
-      </c>
-      <c r="I31" s="4">
-        <v>60</v>
-      </c>
-      <c r="J31" s="4">
-        <v>60</v>
-      </c>
-      <c r="K31" s="4">
-        <v>60</v>
-      </c>
-      <c r="L31" s="4">
-        <v>60</v>
-      </c>
-      <c r="M31" s="4">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>16</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D32">
-        <v>295</v>
-      </c>
-      <c r="E32">
-        <v>295</v>
-      </c>
-      <c r="F32">
-        <v>295</v>
-      </c>
-      <c r="G32">
-        <v>295</v>
-      </c>
-      <c r="H32">
-        <v>295</v>
-      </c>
-      <c r="I32">
-        <v>295</v>
-      </c>
-      <c r="J32">
-        <v>295</v>
-      </c>
-      <c r="K32">
-        <v>295</v>
-      </c>
-      <c r="L32">
-        <v>295</v>
-      </c>
-      <c r="M32">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>80</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D33">
-        <v>40</v>
-      </c>
-      <c r="E33">
-        <v>40</v>
-      </c>
-      <c r="F33">
-        <v>40</v>
-      </c>
-      <c r="G33">
-        <v>40</v>
-      </c>
-      <c r="H33">
-        <v>40</v>
-      </c>
-      <c r="I33">
-        <v>40</v>
-      </c>
-      <c r="J33">
-        <v>40</v>
-      </c>
-      <c r="K33">
-        <v>40</v>
-      </c>
-      <c r="L33">
-        <v>40</v>
-      </c>
-      <c r="M33">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>61</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="D34" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="E34" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="F34" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="G34" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="H34" t="s">
-        <v>63</v>
-      </c>
-      <c r="I34" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="J34" s="7" t="s">
-        <v>64</v>
+        <v>46</v>
+      </c>
+      <c r="I34" t="s">
+        <v>46</v>
+      </c>
+      <c r="J34" t="s">
+        <v>46</v>
       </c>
       <c r="K34" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="L34" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="M34" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>33</v>
+        <v>46</v>
+      </c>
+      <c r="N34" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>42</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>21</v>
@@ -2051,104 +2186,24 @@
       <c r="C35" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E35" t="s">
-        <v>43</v>
-      </c>
-      <c r="F35" t="s">
-        <v>43</v>
-      </c>
-      <c r="G35" t="s">
-        <v>43</v>
-      </c>
-      <c r="H35" t="s">
-        <v>43</v>
-      </c>
-      <c r="I35" t="s">
-        <v>43</v>
-      </c>
-      <c r="J35" t="s">
-        <v>43</v>
+      <c r="D35" t="s">
+        <v>50</v>
       </c>
       <c r="K35" t="s">
-        <v>43</v>
-      </c>
-      <c r="L35" t="s">
-        <v>43</v>
-      </c>
-      <c r="M35" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D36" t="s">
-        <v>46</v>
-      </c>
-      <c r="E36" t="s">
-        <v>46</v>
-      </c>
-      <c r="F36" t="s">
-        <v>46</v>
-      </c>
-      <c r="G36" t="s">
-        <v>46</v>
-      </c>
-      <c r="H36" t="s">
-        <v>46</v>
-      </c>
-      <c r="I36" t="s">
-        <v>46</v>
-      </c>
-      <c r="J36" t="s">
-        <v>46</v>
-      </c>
-      <c r="K36" t="s">
-        <v>46</v>
-      </c>
-      <c r="L36" t="s">
-        <v>46</v>
-      </c>
-      <c r="M36" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>42</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D37" t="s">
-        <v>50</v>
-      </c>
-      <c r="K37" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>75</v>
-      </c>
-      <c r="I38" s="9"/>
-      <c r="J38" s="9"/>
-      <c r="K38" s="9"/>
-      <c r="L38" s="9"/>
-      <c r="M38" s="9"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>73</v>
+      </c>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="9"/>
+      <c r="L36" s="9"/>
+      <c r="M36" s="9"/>
+      <c r="N36" s="9"/>
+      <c r="O36" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
validation + better azimuth
</commit_message>
<xml_diff>
--- a/reskit/solar/workflows/CSP_data/CSP_database.xlsx
+++ b/reskit/solar/workflows/CSP_data/CSP_database.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d.franzmann\Code\RESKit\reskit\solar\workflows\CSP_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E7A981-2C4F-4D76-9A5A-B0FD5656DD8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68443B6-4D6E-45DB-B30B-E6907775190F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16920" xr2:uid="{EF8FF396-6CE6-4D67-BA8C-A21BECB15794}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="122">
   <si>
     <t>Parameter</t>
   </si>
@@ -318,9 +318,6 @@
     <t>SONG, Y. Q., Y. XIANG, Y. B. LIAO, B. ZHANG, L. WU, and H. T. ZHANG. How to decide the alignment of the parabolic trough collector according to the local latitude. 2013 International Conference on Materials for Renewable Energy and Environment (ICMREE 2013). Chengdu, China, 19 - 21 August 2013 ; [proceedings. Piscataway, NJ: IEEE, 2013, pp. 94-97.</t>
   </si>
   <si>
-    <t>Assumed / fits with most plants in: SOLARPACES. CSP Projects Around the World [online] [viewed 10 June 2021]. Available from: https://www.solarpaces.org/csp-technologies/csp-projects-around-the-world/.</t>
-  </si>
-  <si>
     <t>GAFUROV, Tokhir, Julio USAOLA, and Milan PRODANOVIC. Modelling of concentrating solar power plant for power system reliability studies [online]. IET Renewable Power Generation. 2015, 9(2), 120-130. Available from: 10.1049/iet-rpg.2013.0377.</t>
   </si>
   <si>
@@ -388,6 +385,21 @@
   </si>
   <si>
     <t>%</t>
+  </si>
+  <si>
+    <t>Assumed / fits with most plants in: SOLARPACES. CSP Projects Around the World [online] [viewed 10 June 2021]. Available from: https://www.solarpaces.org/csp-technologies/csp-projects-around-the-world/, also to greenius default values</t>
+  </si>
+  <si>
+    <t>Dataset_Heliosol_2030_eastwest</t>
+  </si>
+  <si>
+    <t>eastwest</t>
+  </si>
+  <si>
+    <t>Dataset_SolarSalt_2030_validation</t>
+  </si>
+  <si>
+    <t>Dataset_Heliosol_2030_validation</t>
   </si>
 </sst>
 </file>
@@ -801,13 +813,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40AE3422-B05C-445F-BBB4-0860483AF0A6}">
-  <dimension ref="A1:S45"/>
+  <dimension ref="A1:V45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="L27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="Q3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N43" sqref="N43"/>
+      <selection pane="bottomRight" activeCell="V7" sqref="V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,10 +832,12 @@
     <col min="8" max="8" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="13" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="18" width="27.5703125" customWidth="1"/>
-    <col min="19" max="19" width="59.7109375" customWidth="1"/>
+    <col min="19" max="19" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="27.5703125" customWidth="1"/>
+    <col min="22" max="22" width="59.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -870,19 +884,28 @@
         <v>80</v>
       </c>
       <c r="P1" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q1" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="R1" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="S1" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="T1" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="Q1" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="R1" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="S1" t="s">
+      <c r="U1" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="V1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>48</v>
       </c>
@@ -932,10 +955,19 @@
         <v>80</v>
       </c>
       <c r="R2" s="15" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="S2" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="T2" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="U2" s="15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -984,17 +1016,26 @@
       <c r="P3" t="s">
         <v>18</v>
       </c>
-      <c r="Q3" s="15" t="s">
+      <c r="Q3" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="R3" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="S3" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="T3" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="R3" s="15" t="s">
+      <c r="U3" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="S3" t="s">
+      <c r="V3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1038,22 +1079,31 @@
         <v>8.4924000000000002E-5</v>
       </c>
       <c r="O4" s="1">
-        <v>-8.7266462599716482E-5</v>
+        <v>8.7266462599716496E-5</v>
       </c>
       <c r="P4" s="1">
-        <v>-8.7266462599716482E-5</v>
+        <v>8.7266462599716496E-5</v>
       </c>
       <c r="Q4" s="16">
-        <v>-8.7266462599716482E-5</v>
+        <v>8.7266462599716496E-5</v>
       </c>
       <c r="R4" s="16">
-        <v>-8.7266462599716482E-5</v>
-      </c>
-      <c r="S4" t="s">
+        <v>8.7266462599716496E-5</v>
+      </c>
+      <c r="S4" s="16">
+        <v>8.7266462599716496E-5</v>
+      </c>
+      <c r="T4" s="16">
+        <v>8.7266462599716496E-5</v>
+      </c>
+      <c r="U4" s="16">
+        <v>8.7266462599716496E-5</v>
+      </c>
+      <c r="V4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1097,22 +1147,31 @@
         <v>3.1093000000000002E-5</v>
       </c>
       <c r="O5" s="1">
-        <v>-3.1070976818244271E-5</v>
+        <v>3.1070976818244299E-5</v>
       </c>
       <c r="P5" s="1">
-        <v>-3.1070976818244271E-5</v>
+        <v>3.1070976818244299E-5</v>
       </c>
       <c r="Q5" s="16">
-        <v>-3.1070976818244271E-5</v>
+        <v>3.1070976818244299E-5</v>
       </c>
       <c r="R5" s="16">
-        <v>-3.1070976818244271E-5</v>
-      </c>
-      <c r="S5" t="s">
+        <v>3.1070976818244299E-5</v>
+      </c>
+      <c r="S5" s="16">
+        <v>3.1070976818244299E-5</v>
+      </c>
+      <c r="T5" s="16">
+        <v>3.1070976818244299E-5</v>
+      </c>
+      <c r="U5" s="16">
+        <v>3.1070976818244299E-5</v>
+      </c>
+      <c r="V5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1167,11 +1226,20 @@
       <c r="R6" s="15">
         <v>0</v>
       </c>
-      <c r="S6" t="s">
+      <c r="S6" s="15">
+        <v>0</v>
+      </c>
+      <c r="T6" s="15">
+        <v>0</v>
+      </c>
+      <c r="U6" s="15">
+        <v>0</v>
+      </c>
+      <c r="V6" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1221,16 +1289,25 @@
         <v>0.82699999999999996</v>
       </c>
       <c r="Q7" s="15">
+        <v>0.92688000000000004</v>
+      </c>
+      <c r="R7" s="15">
+        <v>0.92688000000000004</v>
+      </c>
+      <c r="S7" s="15">
+        <v>0.92688000000000004</v>
+      </c>
+      <c r="T7" s="15">
         <v>0.82699999999999996</v>
       </c>
-      <c r="R7" s="15">
+      <c r="U7" s="15">
         <v>0.82699999999999996</v>
       </c>
-      <c r="S7" t="s">
+      <c r="V7" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1256,8 +1333,17 @@
       <c r="R8" s="15">
         <v>-1</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S8" s="15">
+        <v>-1</v>
+      </c>
+      <c r="T8" s="15">
+        <v>-1</v>
+      </c>
+      <c r="U8" s="15">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1312,11 +1398,20 @@
       <c r="R9" s="15">
         <v>16</v>
       </c>
-      <c r="S9" t="s">
+      <c r="S9" s="15">
+        <v>16</v>
+      </c>
+      <c r="T9" s="15">
+        <v>16</v>
+      </c>
+      <c r="U9" s="15">
+        <v>16</v>
+      </c>
+      <c r="V9" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1371,11 +1466,20 @@
       <c r="R10" s="15">
         <v>0</v>
       </c>
-      <c r="S10" t="s">
+      <c r="S10" s="15">
+        <v>0</v>
+      </c>
+      <c r="T10" s="15">
+        <v>0</v>
+      </c>
+      <c r="U10" s="15">
+        <v>0</v>
+      </c>
+      <c r="V10" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1428,13 +1532,22 @@
         <v>4.4701935910452829E-2</v>
       </c>
       <c r="R11" s="15">
+        <v>4.4701935910452802E-2</v>
+      </c>
+      <c r="S11" s="15">
+        <v>4.4701935910452802E-2</v>
+      </c>
+      <c r="T11" s="15">
         <v>4.4701935910452829E-2</v>
       </c>
-      <c r="S11" t="s">
+      <c r="U11" s="15">
+        <v>4.4701935910452802E-2</v>
+      </c>
+      <c r="V11" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1489,11 +1602,20 @@
       <c r="R12" s="15">
         <v>-2.9278818932777496E-4</v>
       </c>
-      <c r="S12" t="s">
+      <c r="S12" s="15">
+        <v>-2.9278818932777496E-4</v>
+      </c>
+      <c r="T12" s="15">
+        <v>-2.9278818932777496E-4</v>
+      </c>
+      <c r="U12" s="15">
+        <v>-2.9278818932777496E-4</v>
+      </c>
+      <c r="V12" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1548,11 +1670,20 @@
       <c r="R13" s="15">
         <v>1.2085236947426394E-6</v>
       </c>
-      <c r="S13" t="s">
+      <c r="S13" s="15">
+        <v>1.2085236947426394E-6</v>
+      </c>
+      <c r="T13" s="15">
+        <v>1.2085236947426394E-6</v>
+      </c>
+      <c r="U13" s="15">
+        <v>1.2085236947426394E-6</v>
+      </c>
+      <c r="V13" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1607,11 +1738,20 @@
       <c r="R14" s="15">
         <v>-4.6531969642924003E-10</v>
       </c>
-      <c r="S14" t="s">
+      <c r="S14" s="15">
+        <v>-4.6531969642924003E-10</v>
+      </c>
+      <c r="T14" s="15">
+        <v>-4.6531969642924003E-10</v>
+      </c>
+      <c r="U14" s="15">
+        <v>-4.6531969642924003E-10</v>
+      </c>
+      <c r="V14" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -1659,15 +1799,24 @@
         <v>1200000</v>
       </c>
       <c r="Q15" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="R15" s="15" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="S15" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="T15" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="U15" s="15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B16" s="3">
         <v>1</v>
@@ -1718,10 +1867,19 @@
       <c r="R16" s="15">
         <v>0.38</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S16" s="15">
+        <v>0.38</v>
+      </c>
+      <c r="T16" s="15">
+        <v>0.38</v>
+      </c>
+      <c r="U16" s="15">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B17" s="3">
         <v>1</v>
@@ -1772,8 +1930,17 @@
       <c r="R17" s="15">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S17" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="T17" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="U17" s="15">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -1829,8 +1996,17 @@
       <c r="R18" s="10">
         <v>-1</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S18" s="10">
+        <v>-1</v>
+      </c>
+      <c r="T18" s="10">
+        <v>-1</v>
+      </c>
+      <c r="U18" s="10">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -1885,11 +2061,20 @@
       <c r="R19" s="15">
         <v>0.96</v>
       </c>
-      <c r="S19" t="s">
+      <c r="S19" s="15">
+        <v>0.96</v>
+      </c>
+      <c r="T19" s="15">
+        <v>0.96</v>
+      </c>
+      <c r="U19" s="15">
+        <v>0.96</v>
+      </c>
+      <c r="V19" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>53</v>
       </c>
@@ -1944,11 +2129,20 @@
       <c r="R20">
         <v>0.108</v>
       </c>
-      <c r="S20" t="s">
+      <c r="S20">
+        <v>0.108</v>
+      </c>
+      <c r="T20">
+        <v>0.108</v>
+      </c>
+      <c r="U20">
+        <v>0.108</v>
+      </c>
+      <c r="V20" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>76</v>
       </c>
@@ -2003,11 +2197,20 @@
       <c r="R21" s="16">
         <v>0</v>
       </c>
-      <c r="S21" t="s">
+      <c r="S21" s="16">
+        <v>0</v>
+      </c>
+      <c r="T21" s="16">
+        <v>0</v>
+      </c>
+      <c r="U21" s="16">
+        <v>0</v>
+      </c>
+      <c r="V21" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>64</v>
       </c>
@@ -2062,11 +2265,20 @@
       <c r="R22" s="15">
         <v>830</v>
       </c>
-      <c r="S22" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S22" s="15">
+        <v>830</v>
+      </c>
+      <c r="T22" s="15">
+        <v>830</v>
+      </c>
+      <c r="U22" s="15">
+        <v>830</v>
+      </c>
+      <c r="V22" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>65</v>
       </c>
@@ -2121,11 +2333,20 @@
       <c r="R23" s="7">
         <v>5.4999999999999997E-3</v>
       </c>
-      <c r="S23" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S23" s="7">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="T23" s="7">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="U23" s="7">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="V23" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>66</v>
       </c>
@@ -2180,11 +2401,20 @@
       <c r="R24" s="7">
         <v>2.5999999999999999E-3</v>
       </c>
-      <c r="S24" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S24" s="7">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="T24" s="7">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="U24" s="7">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="V24" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>67</v>
       </c>
@@ -2239,11 +2469,20 @@
       <c r="R25" s="7">
         <v>0.05</v>
       </c>
-      <c r="S25" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S25" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="T25" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="U25" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="V25" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>68</v>
       </c>
@@ -2298,11 +2537,20 @@
       <c r="R26" s="7">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="S26" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S26" s="7">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="T26" s="7">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="U26" s="7">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="V26" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>69</v>
       </c>
@@ -2357,11 +2605,20 @@
       <c r="R27" s="7">
         <v>1.9E-2</v>
       </c>
-      <c r="S27" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S27" s="7">
+        <v>1.9E-2</v>
+      </c>
+      <c r="T27" s="7">
+        <v>1.9E-2</v>
+      </c>
+      <c r="U27" s="7">
+        <v>1.9E-2</v>
+      </c>
+      <c r="V27" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>50</v>
       </c>
@@ -2411,16 +2668,30 @@
         <v>3688</v>
       </c>
       <c r="Q28" s="7">
-        <v>3688</v>
+        <f>P28*4/3</f>
+        <v>4917.333333333333</v>
       </c>
       <c r="R28" s="7">
-        <v>3688</v>
-      </c>
-      <c r="S28" t="s">
+        <f>P28*10/14</f>
+        <v>2634.2857142857142</v>
+      </c>
+      <c r="S28" s="7">
+        <f>Q28*10/14</f>
+        <v>3512.3809523809518</v>
+      </c>
+      <c r="T28" s="7">
+        <f>S28*4/3</f>
+        <v>4683.1746031746025</v>
+      </c>
+      <c r="U28" s="7">
+        <f>S28*10/14</f>
+        <v>2508.8435374149658</v>
+      </c>
+      <c r="V28" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>13</v>
       </c>
@@ -2475,11 +2746,20 @@
       <c r="R29" s="15">
         <v>405</v>
       </c>
-      <c r="S29" t="s">
+      <c r="S29" s="15">
+        <v>405</v>
+      </c>
+      <c r="T29" s="7">
+        <v>560</v>
+      </c>
+      <c r="U29" s="15">
+        <v>405</v>
+      </c>
+      <c r="V29" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -2534,11 +2814,20 @@
       <c r="R30" s="15">
         <v>-20</v>
       </c>
-      <c r="S30" t="s">
+      <c r="S30" s="15">
+        <v>-20</v>
+      </c>
+      <c r="T30" s="7">
+        <v>260</v>
+      </c>
+      <c r="U30" s="15">
+        <v>-20</v>
+      </c>
+      <c r="V30" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>15</v>
       </c>
@@ -2588,16 +2877,25 @@
         <v>295</v>
       </c>
       <c r="Q31" s="7">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="R31" s="15">
-        <v>295</v>
-      </c>
-      <c r="S31" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="S31" s="15">
+        <v>290</v>
+      </c>
+      <c r="T31" s="7">
+        <v>290</v>
+      </c>
+      <c r="U31" s="15">
+        <v>290</v>
+      </c>
+      <c r="V31" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>77</v>
       </c>
@@ -2652,16 +2950,25 @@
       <c r="R32">
         <v>25</v>
       </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S32">
+        <v>25</v>
+      </c>
+      <c r="T32">
+        <v>25</v>
+      </c>
+      <c r="U32">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D33" s="17">
         <v>1140</v>
@@ -2708,16 +3015,25 @@
       <c r="R33" s="15">
         <v>1140</v>
       </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S33" s="15">
+        <v>1140</v>
+      </c>
+      <c r="T33" s="15">
+        <v>1140</v>
+      </c>
+      <c r="U33" s="15">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D34" s="17">
         <v>29</v>
@@ -2764,16 +3080,25 @@
       <c r="R34" s="15">
         <v>42</v>
       </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S34" s="15">
+        <v>42</v>
+      </c>
+      <c r="T34" s="7">
+        <v>29</v>
+      </c>
+      <c r="U34" s="15">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D35" s="17">
         <v>188</v>
@@ -2820,16 +3145,25 @@
       <c r="R35" s="15">
         <v>219</v>
       </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S35" s="15">
+        <v>219</v>
+      </c>
+      <c r="T35" s="7">
+        <v>188</v>
+      </c>
+      <c r="U35" s="15">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D36" s="17">
         <v>1</v>
@@ -2876,16 +3210,25 @@
       <c r="R36" s="15">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S36" s="15">
+        <v>1</v>
+      </c>
+      <c r="T36" s="7">
+        <v>1</v>
+      </c>
+      <c r="U36" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B37" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>113</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>114</v>
       </c>
       <c r="D37" s="17">
         <v>11</v>
@@ -2932,16 +3275,25 @@
       <c r="R37" s="15">
         <v>11</v>
       </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S37" s="15">
+        <v>11</v>
+      </c>
+      <c r="T37" s="7">
+        <v>11</v>
+      </c>
+      <c r="U37" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B38" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>113</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>114</v>
       </c>
       <c r="D38" s="17">
         <v>2</v>
@@ -2988,16 +3340,25 @@
       <c r="R38" s="15">
         <v>2</v>
       </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S38" s="15">
+        <v>2</v>
+      </c>
+      <c r="T38" s="7">
+        <v>2</v>
+      </c>
+      <c r="U38" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D39" s="17">
         <v>0.04</v>
@@ -3044,16 +3405,25 @@
       <c r="R39" s="15">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S39" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="T39" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="U39" s="15">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>115</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B40" s="3" t="s">
-        <v>117</v>
-      </c>
       <c r="C40" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D40" s="17">
         <v>8</v>
@@ -3100,8 +3470,17 @@
       <c r="R40" s="15">
         <v>8</v>
       </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S40" s="15">
+        <v>8</v>
+      </c>
+      <c r="T40" s="15">
+        <v>8</v>
+      </c>
+      <c r="U40" s="15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>58</v>
       </c>
@@ -3156,8 +3535,17 @@
       <c r="R41" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S41" t="s">
+        <v>60</v>
+      </c>
+      <c r="T41" t="s">
+        <v>60</v>
+      </c>
+      <c r="U41" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>32</v>
       </c>
@@ -3212,8 +3600,17 @@
       <c r="R42" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S42" t="s">
+        <v>42</v>
+      </c>
+      <c r="T42" t="s">
+        <v>42</v>
+      </c>
+      <c r="U42" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>35</v>
       </c>
@@ -3268,8 +3665,17 @@
       <c r="R43" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S43" t="s">
+        <v>90</v>
+      </c>
+      <c r="T43" t="s">
+        <v>90</v>
+      </c>
+      <c r="U43" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>41</v>
       </c>
@@ -3286,7 +3692,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>72</v>
       </c>

</xml_diff>

<commit_message>
small changes in workflow
</commit_message>
<xml_diff>
--- a/reskit/solar/workflows/CSP_data/CSP_database.xlsx
+++ b/reskit/solar/workflows/CSP_data/CSP_database.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d.franzmann\Code\RESKit\reskit\solar\workflows\CSP_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A9A135-9DF7-4387-B08F-6FB72970C84D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F96BB3A4-1808-4646-9E79-C8A6885BF327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16920" xr2:uid="{EF8FF396-6CE6-4D67-BA8C-A21BECB15794}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="123">
   <si>
     <t>Parameter</t>
   </si>
@@ -400,6 +400,9 @@
   </si>
   <si>
     <t>Dataset_Heliosol_2030_validation</t>
+  </si>
+  <si>
+    <t>Heliosol</t>
   </si>
 </sst>
 </file>
@@ -819,7 +822,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="Q3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Q20" sqref="Q20"/>
+      <selection pane="bottomRight" activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1288,13 +1291,13 @@
       <c r="P7">
         <v>0.82699999999999996</v>
       </c>
-      <c r="Q7" s="15">
+      <c r="Q7" s="13">
         <v>0.92688000000000004</v>
       </c>
-      <c r="R7" s="15">
+      <c r="R7" s="13">
         <v>0.92688000000000004</v>
       </c>
-      <c r="S7" s="15">
+      <c r="S7" s="13">
         <v>0.92688000000000004</v>
       </c>
       <c r="T7" s="15">
@@ -3663,16 +3666,16 @@
         <v>90</v>
       </c>
       <c r="R43" t="s">
-        <v>90</v>
+        <v>122</v>
       </c>
       <c r="S43" t="s">
-        <v>90</v>
+        <v>122</v>
       </c>
       <c r="T43" t="s">
         <v>90</v>
       </c>
       <c r="U43" t="s">
-        <v>90</v>
+        <v>122</v>
       </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">

</xml_diff>